<commit_message>
Para produccion - Externo
</commit_message>
<xml_diff>
--- a/importar/preguntas.xlsx
+++ b/importar/preguntas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moren\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2850F-95E0-4150-8DF9-2D60364ABAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA51482F-0041-4B9D-8738-3443DE6EBC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4227,8 +4227,8 @@
   <dimension ref="A1:I349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G327" sqref="G327"/>
+      <pane ySplit="1" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>